<commit_message>
coded complexity items into morphology/syntax
</commit_message>
<xml_diff>
--- a/raw_data/English_WG/[English_WG].xlsx
+++ b/raw_data/English_WG/[English_WG].xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3560" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3561" uniqueCount="583">
   <si>
     <t>sounds</t>
   </si>
@@ -1765,6 +1765,9 @@
   </si>
   <si>
     <t>descriptive_words</t>
+  </si>
+  <si>
+    <t>complexity_category</t>
   </si>
 </sst>
 </file>
@@ -2355,10 +2358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1743"/>
+  <dimension ref="A1:I1743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B421" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C397" sqref="C397"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2372,7 +2375,7 @@
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>446</v>
       </c>
@@ -2397,8 +2400,11 @@
       <c r="H1" s="2" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="13" t="s">
         <v>449</v>
       </c>
@@ -2415,7 +2421,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
         <v>450</v>
       </c>
@@ -2432,7 +2438,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="13" t="s">
         <v>451</v>
       </c>
@@ -2449,7 +2455,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="13" t="s">
         <v>452</v>
       </c>
@@ -2466,7 +2472,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
         <v>453</v>
       </c>
@@ -2483,7 +2489,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
         <v>454</v>
       </c>
@@ -2500,7 +2506,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
         <v>455</v>
       </c>
@@ -2517,7 +2523,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="13" t="s">
         <v>456</v>
       </c>
@@ -2534,7 +2540,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="13" t="s">
         <v>457</v>
       </c>
@@ -2551,7 +2557,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="13" t="s">
         <v>458</v>
       </c>
@@ -2568,7 +2574,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="13" t="s">
         <v>459</v>
       </c>
@@ -2585,7 +2591,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="13" t="s">
         <v>460</v>
       </c>
@@ -2602,7 +2608,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="13" t="s">
         <v>461</v>
       </c>
@@ -2619,7 +2625,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="13" t="s">
         <v>462</v>
       </c>
@@ -2636,7 +2642,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="13" t="s">
         <v>463</v>
       </c>

</xml_diff>

<commit_message>
Spanish WG uni_lemma mapping
</commit_message>
<xml_diff>
--- a/raw_data/English_WG/[English_WG].xlsx
+++ b/raw_data/English_WG/[English_WG].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19900" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1072">
   <si>
     <t>sounds</t>
   </si>
@@ -3232,6 +3232,9 @@
   </si>
   <si>
     <t>night night</t>
+  </si>
+  <si>
+    <t>comb (object)</t>
   </si>
 </sst>
 </file>
@@ -3906,8 +3909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A269" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8917,7 +8920,7 @@
         <v>1065</v>
       </c>
       <c r="F200" s="19" t="s">
-        <v>139</v>
+        <v>1071</v>
       </c>
       <c r="G200" s="19" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
a little (description) fix
</commit_message>
<xml_diff>
--- a/raw_data/English_WG/[English_WG].xlsx
+++ b/raw_data/English_WG/[English_WG].xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="1073">
   <si>
     <t>sounds</t>
   </si>
@@ -3235,6 +3235,9 @@
   </si>
   <si>
     <t>comb (object)</t>
+  </si>
+  <si>
+    <t>little (description)</t>
   </si>
 </sst>
 </file>
@@ -3342,8 +3345,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3495,7 +3500,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3537,6 +3542,7 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3578,6 +3584,7 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3909,8 +3916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A269" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B364" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B381" sqref="B381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13626,13 +13633,13 @@
         <v>1065</v>
       </c>
       <c r="F381" s="19" t="s">
-        <v>300</v>
+        <v>1072</v>
       </c>
       <c r="G381" s="19" t="s">
-        <v>300</v>
+        <v>1072</v>
       </c>
       <c r="H381" s="19" t="s">
-        <v>300</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="382" spans="1:8">

</xml_diff>